<commit_message>
Added support for new Excel file structure
</commit_message>
<xml_diff>
--- a/AutomationTest/PPJ rettigheder - alle tildelinger.xlsx
+++ b/AutomationTest/PPJ rettigheder - alle tildelinger.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="42940" windowHeight="20720" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="2" r:id="rId1"/>
@@ -362,9 +362,6 @@
     <t>URI prefix</t>
   </si>
   <si>
-    <t>urn:dsdn:ppj:</t>
-  </si>
-  <si>
     <t>Kort navn</t>
   </si>
   <si>
@@ -513,13 +510,16 @@
   </si>
   <si>
     <t>Rolle 130</t>
+  </si>
+  <si>
+    <t>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,13 +621,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -711,17 +704,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -853,15 +847,15 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -871,6 +865,7 @@
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1141,7 +1136,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1219,14 +1214,14 @@
   <dimension ref="A1:AA77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B44" sqref="B44:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="44.5" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="64" customWidth="1"/>
     <col min="4" max="4" width="70.1640625" style="10" customWidth="1"/>
     <col min="5" max="5" width="86.6640625" style="9" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" style="8" customWidth="1"/>
@@ -1235,10 +1230,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="39" customHeight="1">
       <c r="C1" s="15"/>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="16"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -1267,7 +1262,7 @@
         <v>106</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>97</v>
@@ -1288,13 +1283,13 @@
         <v>44</v>
       </c>
       <c r="J2" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="K2" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="19" t="s">
         <v>157</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>158</v>
       </c>
       <c r="M2" s="19"/>
       <c r="N2" s="20"/>
@@ -1349,25 +1344,25 @@
       <c r="D4" s="27"/>
       <c r="E4" s="28"/>
       <c r="F4" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
@@ -1387,11 +1382,11 @@
     </row>
     <row r="5" spans="1:27">
       <c r="B5" s="41" t="str">
-        <f t="shared" ref="B5:B26" si="0">IF(LEN(D5)&gt;0,CONCATENATE( C$77,C5),"")</f>
-        <v>urn:dsdn:ppj:LoggePaaMobilEnhed</v>
+        <f>IF(LEN(D5)&gt;0,CONCATENATE( C$77,"ppj"),"")</f>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>25</v>
@@ -1400,25 +1395,25 @@
         <v>45</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K5" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
@@ -1438,11 +1433,11 @@
     </row>
     <row r="6" spans="1:27">
       <c r="B6" s="41" t="str">
-        <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:RedigereAktiveJournalerTilKnyttetAktuelleHaendelse</v>
+        <f t="shared" ref="B6:B69" si="0">IF(LEN(D6)&gt;0,CONCATENATE( C$77,"ppj"),"")</f>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>6</v>
@@ -1451,25 +1446,25 @@
         <v>46</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
@@ -1496,25 +1491,25 @@
       <c r="D7" s="33"/>
       <c r="E7" s="34"/>
       <c r="F7" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -1535,10 +1530,10 @@
     <row r="8" spans="1:27">
       <c r="B8" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:SeEgneTidligereJournaler</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>22</v>
@@ -1547,25 +1542,25 @@
         <v>47</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
@@ -1586,10 +1581,10 @@
     <row r="9" spans="1:27">
       <c r="B9" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:RedigereEgneTidligereJournaler</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>23</v>
@@ -1598,25 +1593,25 @@
         <v>50</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L9" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
@@ -1637,10 +1632,10 @@
     <row r="10" spans="1:27">
       <c r="B10" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:RedigereTidligereJounaler</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>48</v>
@@ -1649,25 +1644,25 @@
         <v>49</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
@@ -1694,25 +1689,25 @@
       <c r="D11" s="33"/>
       <c r="E11" s="34"/>
       <c r="F11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L11" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
@@ -1733,10 +1728,10 @@
     <row r="12" spans="1:27">
       <c r="B12" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:SoegeEfterTidligereJournalerForAktuellePatient</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>18</v>
@@ -1745,25 +1740,25 @@
         <v>96</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K12" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L12" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -1784,10 +1779,10 @@
     <row r="13" spans="1:27">
       <c r="B13" s="41" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">urn:dsdn:ppj:SoegeEfterEgneTidligereJournaler </v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>19</v>
@@ -1796,25 +1791,25 @@
         <v>95</v>
       </c>
       <c r="F13" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K13" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L13" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
@@ -1841,25 +1836,25 @@
       <c r="D14" s="33"/>
       <c r="E14" s="34"/>
       <c r="F14" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
@@ -1880,10 +1875,10 @@
     <row r="15" spans="1:27">
       <c r="B15" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:OpretteBehandlingsplads</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>37</v>
@@ -1892,25 +1887,25 @@
         <v>51</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I15" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K15" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L15" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
@@ -1931,10 +1926,10 @@
     <row r="16" spans="1:27">
       <c r="B16" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:VisningAfBehandlingspladsTilknyttetAktuelHaendelse</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D16" s="33" t="s">
         <v>38</v>
@@ -1943,25 +1938,25 @@
         <v>52</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M16" s="15"/>
       <c r="N16" s="15"/>
@@ -1988,25 +1983,25 @@
       <c r="D17" s="33"/>
       <c r="E17" s="34"/>
       <c r="F17" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K17" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
@@ -2027,10 +2022,10 @@
     <row r="18" spans="1:27">
       <c r="B18" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:AdgangTilFMKInformationForAktuellePatient</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>7</v>
@@ -2039,25 +2034,25 @@
         <v>94</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
@@ -2078,10 +2073,10 @@
     <row r="19" spans="1:27">
       <c r="B19" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:AdgangTilE-JournalForAktuellePatient</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C19" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>24</v>
@@ -2090,25 +2085,25 @@
         <v>53</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H19" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J19" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K19" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L19" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
@@ -2135,25 +2130,25 @@
       <c r="D20" s="31"/>
       <c r="E20" s="32"/>
       <c r="F20" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J20" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K20" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L20" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
@@ -2174,10 +2169,10 @@
     <row r="21" spans="1:27">
       <c r="B21" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:RegistreringAfMedicinklasse1</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>0</v>
@@ -2186,25 +2181,25 @@
         <v>54</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H21" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K21" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L21" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
@@ -2225,10 +2220,10 @@
     <row r="22" spans="1:27">
       <c r="B22" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:RegistreringAfMedicinklasse2</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>1</v>
@@ -2237,25 +2232,25 @@
         <v>55</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H22" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J22" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K22" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L22" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
@@ -2276,10 +2271,10 @@
     <row r="23" spans="1:27">
       <c r="B23" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:RegistreringAfMedicinklasse3</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>2</v>
@@ -2288,25 +2283,25 @@
         <v>56</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H23" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J23" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K23" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L23" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
@@ -2333,25 +2328,25 @@
       <c r="D24" s="31"/>
       <c r="E24" s="37"/>
       <c r="F24" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H24" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I24" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J24" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K24" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L24" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M24" s="15"/>
       <c r="N24" s="15"/>
@@ -2372,10 +2367,10 @@
     <row r="25" spans="1:27">
       <c r="B25" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:OpslagAfNavnAdresseFraCPR</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>16</v>
@@ -2384,25 +2379,25 @@
         <v>57</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L25" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
@@ -2423,10 +2418,10 @@
     <row r="26" spans="1:27">
       <c r="B26" s="41" t="str">
         <f t="shared" si="0"/>
-        <v>urn:dsdn:ppj:OpslagAfCPRFraNavnAdresseKoen</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D26" s="31" t="s">
         <v>17</v>
@@ -2435,25 +2430,25 @@
         <v>58</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L26" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
@@ -2477,25 +2472,25 @@
       <c r="D27" s="31"/>
       <c r="E27" s="32"/>
       <c r="F27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L27" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
@@ -2519,25 +2514,25 @@
       <c r="D28" s="31"/>
       <c r="E28" s="32"/>
       <c r="F28" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J28" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K28" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L28" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
@@ -2564,25 +2559,25 @@
       <c r="D29" s="23"/>
       <c r="E29" s="24"/>
       <c r="F29" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H29" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I29" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J29" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K29" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L29" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
@@ -2606,25 +2601,25 @@
       <c r="D30" s="31"/>
       <c r="E30" s="32"/>
       <c r="F30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L30" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M30" s="15"/>
       <c r="N30" s="15"/>
@@ -2644,11 +2639,11 @@
     </row>
     <row r="31" spans="1:27">
       <c r="B31" s="41" t="str">
-        <f t="shared" ref="B31:B75" si="1">IF(LEN(D31)&gt;0,CONCATENATE( C$77,C31),"")</f>
-        <v>urn:dsdn:ppj:LoggePaaCentralPPJ</v>
+        <f>IF(LEN(D31)&gt;0,CONCATENATE( C$77,"ppj"),"")</f>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D31" s="31" t="s">
         <v>39</v>
@@ -2657,25 +2652,25 @@
         <v>59</v>
       </c>
       <c r="F31" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H31" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I31" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J31" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K31" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L31" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
@@ -2695,32 +2690,32 @@
     </row>
     <row r="32" spans="1:27">
       <c r="B32" s="41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B32:B75" si="1">IF(LEN(D32)&gt;0,CONCATENATE( C$77,"ppj"),"")</f>
         <v/>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="31"/>
       <c r="E32" s="32"/>
       <c r="F32" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G32" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H32" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J32" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K32" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L32" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
@@ -2741,10 +2736,10 @@
     <row r="33" spans="2:27">
       <c r="B33" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAktiveHaendelserForEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>103</v>
@@ -2753,25 +2748,25 @@
         <v>104</v>
       </c>
       <c r="F33" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G33" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H33" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I33" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J33" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K33" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L33" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
@@ -2798,25 +2793,25 @@
       <c r="D34" s="38"/>
       <c r="E34" s="32"/>
       <c r="F34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L34" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
@@ -2837,10 +2832,10 @@
     <row r="35" spans="2:27">
       <c r="B35" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAlleAktiveJournalerIEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="33" t="s">
         <v>13</v>
@@ -2849,25 +2844,25 @@
         <v>60</v>
       </c>
       <c r="F35" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G35" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H35" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I35" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J35" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K35" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L35" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
@@ -2888,10 +2883,10 @@
     <row r="36" spans="2:27">
       <c r="B36" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAlleTidligereJournalerIEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D36" s="33" t="s">
         <v>12</v>
@@ -2900,25 +2895,25 @@
         <v>61</v>
       </c>
       <c r="F36" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G36" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H36" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I36" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J36" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K36" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
@@ -2945,25 +2940,25 @@
       <c r="D37" s="33"/>
       <c r="E37" s="34"/>
       <c r="F37" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G37" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H37" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I37" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J37" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K37" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L37" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
@@ -2984,10 +2979,10 @@
     <row r="38" spans="2:27">
       <c r="B38" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAlleJournalerMedEKGIEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D38" s="33" t="s">
         <v>93</v>
@@ -2996,25 +2991,25 @@
         <v>92</v>
       </c>
       <c r="F38" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G38" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H38" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I38" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J38" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K38" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L38" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
@@ -3041,25 +3036,25 @@
       <c r="D39" s="33"/>
       <c r="E39" s="34"/>
       <c r="F39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L39" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
@@ -3080,10 +3075,10 @@
     <row r="40" spans="2:27" ht="30">
       <c r="B40" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAlleAktiveJournalerPaaVejModEgenModtagelse</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D40" s="33" t="s">
         <v>11</v>
@@ -3092,25 +3087,25 @@
         <v>91</v>
       </c>
       <c r="F40" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G40" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H40" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I40" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J40" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K40" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L40" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M40" s="15"/>
       <c r="N40" s="15"/>
@@ -3131,10 +3126,10 @@
     <row r="41" spans="2:27" ht="30">
       <c r="B41" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAlleTidligereJournalerTilEgenModtagelse</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D41" s="31" t="s">
         <v>10</v>
@@ -3143,25 +3138,25 @@
         <v>90</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G41" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H41" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I41" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J41" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K41" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L41" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
@@ -3188,25 +3183,25 @@
       <c r="D42" s="31"/>
       <c r="E42" s="32"/>
       <c r="F42" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G42" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H42" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I42" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J42" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K42" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L42" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
@@ -3227,10 +3222,10 @@
     <row r="43" spans="2:27" ht="30">
       <c r="B43" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAktiveJournalerTilEgenRegionUdenModtagelse</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C43" s="35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D43" s="31" t="s">
         <v>3</v>
@@ -3239,25 +3234,25 @@
         <v>89</v>
       </c>
       <c r="F43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
@@ -3278,10 +3273,10 @@
     <row r="44" spans="2:27" ht="30">
       <c r="B44" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeTidligereJournalerTilEgenRegionUdenModtagelse</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D44" s="31" t="s">
         <v>26</v>
@@ -3290,25 +3285,25 @@
         <v>88</v>
       </c>
       <c r="F44" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G44" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H44" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I44" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J44" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K44" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L44" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
@@ -3335,25 +3330,25 @@
       <c r="D45" s="31"/>
       <c r="E45" s="32"/>
       <c r="F45" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G45" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J45" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K45" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L45" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
@@ -3374,10 +3369,10 @@
     <row r="46" spans="2:27">
       <c r="B46" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeJournalerAfsluttetPaaStedet</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C46" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D46" s="31" t="s">
         <v>27</v>
@@ -3386,25 +3381,25 @@
         <v>87</v>
       </c>
       <c r="F46" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H46" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J46" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K46" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L46" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
@@ -3431,25 +3426,25 @@
       <c r="D47" s="31"/>
       <c r="E47" s="32"/>
       <c r="F47" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G47" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H47" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J47" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K47" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L47" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
@@ -3470,10 +3465,10 @@
     <row r="48" spans="2:27">
       <c r="B48" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:UdfoereTilbagemeldingerPaaJournaler</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D48" s="31" t="s">
         <v>35</v>
@@ -3482,25 +3477,25 @@
         <v>62</v>
       </c>
       <c r="F48" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G48" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H48" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J48" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K48" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L48" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
@@ -3521,10 +3516,10 @@
     <row r="49" spans="2:27">
       <c r="B49" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeAlleTilbagemeldingerIndenforEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D49" s="31" t="s">
         <v>36</v>
@@ -3533,25 +3528,25 @@
         <v>63</v>
       </c>
       <c r="F49" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G49" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H49" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I49" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J49" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K49" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L49" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M49" s="15"/>
       <c r="N49" s="15"/>
@@ -3578,25 +3573,25 @@
       <c r="D50" s="31"/>
       <c r="E50" s="32"/>
       <c r="F50" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G50" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H50" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I50" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J50" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K50" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L50" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
@@ -3617,10 +3612,10 @@
     <row r="51" spans="2:27">
       <c r="B51" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeBehandlerpladslogForEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C51" s="35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D51" s="31" t="s">
         <v>8</v>
@@ -3629,25 +3624,25 @@
         <v>64</v>
       </c>
       <c r="F51" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I51" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J51" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K51" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L51" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
@@ -3668,10 +3663,10 @@
     <row r="52" spans="2:27">
       <c r="B52" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:RedigereBhandlerpladsForEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C52" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D52" s="31" t="s">
         <v>9</v>
@@ -3680,25 +3675,25 @@
         <v>65</v>
       </c>
       <c r="F52" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G52" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H52" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I52" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J52" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K52" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L52" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M52" s="15"/>
       <c r="N52" s="15"/>
@@ -3719,10 +3714,10 @@
     <row r="53" spans="2:27">
       <c r="B53" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:AngiveKapaciteterForModtagelserIEgenRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C53" s="35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D53" s="31" t="s">
         <v>20</v>
@@ -3731,25 +3726,25 @@
         <v>66</v>
       </c>
       <c r="F53" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G53" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H53" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I53" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J53" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K53" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L53" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -3776,25 +3771,25 @@
       <c r="D54" s="31"/>
       <c r="E54" s="32"/>
       <c r="F54" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G54" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H54" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I54" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J54" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K54" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L54" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
@@ -3815,10 +3810,10 @@
     <row r="55" spans="2:27">
       <c r="B55" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeEgneJournaler</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C55" s="35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D55" s="31" t="s">
         <v>28</v>
@@ -3827,25 +3822,25 @@
         <v>86</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G55" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H55" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I55" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J55" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K55" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L55" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
@@ -3866,10 +3861,10 @@
     <row r="56" spans="2:27">
       <c r="B56" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeEgenOperatoersJournaler</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C56" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D56" s="31" t="s">
         <v>15</v>
@@ -3878,25 +3873,25 @@
         <v>85</v>
       </c>
       <c r="F56" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G56" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H56" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I56" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J56" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K56" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L56" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
@@ -3917,10 +3912,10 @@
     <row r="57" spans="2:27">
       <c r="B57" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeJournalerFraAlleOperatoererIRegion</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C57" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>29</v>
@@ -3929,25 +3924,25 @@
         <v>84</v>
       </c>
       <c r="F57" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G57" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H57" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I57" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J57" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K57" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L57" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M57" s="15"/>
       <c r="N57" s="15"/>
@@ -3974,25 +3969,25 @@
       <c r="D58" s="31"/>
       <c r="E58" s="32"/>
       <c r="F58" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G58" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H58" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I58" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J58" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K58" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L58" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M58" s="15"/>
       <c r="N58" s="15"/>
@@ -4013,10 +4008,10 @@
     <row r="59" spans="2:27">
       <c r="B59" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SoegeEfterAfsluttedeJournalerUdfraCPR</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D59" s="31" t="s">
         <v>21</v>
@@ -4025,25 +4020,25 @@
         <v>83</v>
       </c>
       <c r="F59" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G59" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H59" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I59" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J59" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K59" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L59" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
@@ -4070,25 +4065,25 @@
       <c r="D60" s="31"/>
       <c r="E60" s="32"/>
       <c r="F60" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G60" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H60" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I60" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J60" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K60" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L60" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M60" s="15"/>
       <c r="N60" s="15"/>
@@ -4109,10 +4104,10 @@
     <row r="61" spans="2:27">
       <c r="B61" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:RegistrerTilbagemeldingerPaaJournalerTilEgenModtagelse</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61" s="31" t="s">
         <v>82</v>
@@ -4121,25 +4116,25 @@
         <v>81</v>
       </c>
       <c r="F61" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G61" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H61" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I61" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J61" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K61" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L61" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M61" s="15"/>
       <c r="N61" s="15"/>
@@ -4160,10 +4155,10 @@
     <row r="62" spans="2:27">
       <c r="B62" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeEgneTilbagemeldinger</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C62" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D62" s="31" t="s">
         <v>14</v>
@@ -4172,25 +4167,25 @@
         <v>68</v>
       </c>
       <c r="F62" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G62" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H62" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I62" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J62" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K62" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L62" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
@@ -4211,10 +4206,10 @@
     <row r="63" spans="2:27">
       <c r="B63" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeTilbagemeldingerTilAndreIndenforEgenOperatoer</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D63" s="31" t="s">
         <v>31</v>
@@ -4223,25 +4218,25 @@
         <v>67</v>
       </c>
       <c r="F63" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G63" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H63" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I63" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J63" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K63" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L63" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
@@ -4268,25 +4263,25 @@
       <c r="D64" s="31"/>
       <c r="E64" s="32"/>
       <c r="F64" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G64" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H64" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I64" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J64" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K64" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L64" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M64" s="15"/>
       <c r="N64" s="15"/>
@@ -4307,10 +4302,10 @@
     <row r="65" spans="2:27">
       <c r="B65" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeEgenKompetencebrug</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D65" s="31" t="s">
         <v>30</v>
@@ -4319,25 +4314,25 @@
         <v>69</v>
       </c>
       <c r="F65" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G65" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H65" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I65" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J65" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K65" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L65" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
@@ -4358,10 +4353,10 @@
     <row r="66" spans="2:27">
       <c r="B66" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeKompetencbrugForAndreIndenforEgenOperatoer</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D66" s="31" t="s">
         <v>32</v>
@@ -4370,25 +4365,25 @@
         <v>70</v>
       </c>
       <c r="F66" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H66" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I66" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J66" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K66" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L66" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M66" s="15"/>
       <c r="N66" s="15"/>
@@ -4415,25 +4410,25 @@
       <c r="D67" s="31"/>
       <c r="E67" s="32"/>
       <c r="F67" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H67" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I67" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J67" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K67" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L67" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M67" s="15"/>
       <c r="N67" s="15"/>
@@ -4454,10 +4449,10 @@
     <row r="68" spans="2:27">
       <c r="B68" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:MaaRedigererStamdata</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C68" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D68" s="31" t="s">
         <v>80</v>
@@ -4466,25 +4461,25 @@
         <v>71</v>
       </c>
       <c r="F68" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G68" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H68" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I68" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J68" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K68" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L68" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
@@ -4511,25 +4506,25 @@
       <c r="D69" s="31"/>
       <c r="E69" s="32"/>
       <c r="F69" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G69" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H69" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J69" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K69" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L69" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
@@ -4550,10 +4545,10 @@
     <row r="70" spans="2:27">
       <c r="B70" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:SeLogFiler</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C70" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D70" s="31" t="s">
         <v>33</v>
@@ -4562,25 +4557,25 @@
         <v>72</v>
       </c>
       <c r="F70" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G70" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H70" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I70" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J70" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K70" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L70" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M70" s="15"/>
       <c r="N70" s="15"/>
@@ -4601,10 +4596,10 @@
     <row r="71" spans="2:27" ht="30">
       <c r="B71" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:Alarmopsaetning</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C71" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D71" s="31" t="s">
         <v>79</v>
@@ -4613,25 +4608,25 @@
         <v>78</v>
       </c>
       <c r="F71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L71" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
@@ -4658,25 +4653,25 @@
       <c r="D72" s="31"/>
       <c r="E72" s="32"/>
       <c r="F72" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G72" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H72" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I72" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J72" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K72" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L72" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
@@ -4697,10 +4692,10 @@
     <row r="73" spans="2:27">
       <c r="B73" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:AdgangTilStatistikDatabaseInterface</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C73" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D73" s="31" t="s">
         <v>34</v>
@@ -4709,25 +4704,25 @@
         <v>73</v>
       </c>
       <c r="F73" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G73" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I73" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J73" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K73" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L73" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
@@ -4754,25 +4749,25 @@
       <c r="D74" s="31"/>
       <c r="E74" s="32"/>
       <c r="F74" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G74" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I74" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J74" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K74" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L74" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M74" s="15"/>
       <c r="N74" s="15"/>
@@ -4793,10 +4788,10 @@
     <row r="75" spans="2:27">
       <c r="B75" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>urn:dsdn:ppj:BrugerAdministration</v>
+        <v>http://schemas.danskeregioner.dk/2013/10/identity/claims/rettighed/ppj</v>
       </c>
       <c r="C75" s="35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D75" s="31" t="s">
         <v>101</v>
@@ -4805,25 +4800,25 @@
         <v>102</v>
       </c>
       <c r="F75" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G75" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H75" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I75" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J75" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K75" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L75" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
@@ -4845,8 +4840,8 @@
       <c r="B77" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C77" s="43" t="s">
-        <v>108</v>
+      <c r="C77" s="44" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4854,6 +4849,9 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C77" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="49" fitToHeight="3" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <extLst>

</xml_diff>